<commit_message>
Correct hydro capacity factor
</commit_message>
<xml_diff>
--- a/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
+++ b/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\BECF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662345F1-5359-4FF9-B020-14A6BD4DE959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5172EBF-D074-4731-B8F0-F57B77384C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,13 @@
     <sheet name="SY_Renewable_Cap" sheetId="17" r:id="rId4"/>
     <sheet name="SY_Renewable_Output" sheetId="16" r:id="rId5"/>
     <sheet name="NREL ATB" sheetId="20" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="21" r:id="rId7"/>
+    <sheet name="Hydro" sheetId="21" r:id="rId7"/>
     <sheet name="StartYear_cal" sheetId="18" r:id="rId8"/>
     <sheet name="BECF-pre-ret" sheetId="4" r:id="rId9"/>
     <sheet name="BECF-pre-nonret" sheetId="5" r:id="rId10"/>
     <sheet name="BECF-new" sheetId="6" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="477">
   <si>
     <t>Source:</t>
   </si>
@@ -1315,6 +1315,213 @@
   </si>
   <si>
     <t>* Data from HIS Markit</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>MWh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Pumped-Storage</t>
+  </si>
+  <si>
+    <t>Small
+hydro</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>1976</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>1973</t>
+  </si>
+  <si>
+    <t>1972</t>
+  </si>
+  <si>
+    <t>1971</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>1969</t>
+  </si>
+  <si>
+    <t>1968</t>
+  </si>
+  <si>
+    <t>1967</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>1965</t>
+  </si>
+  <si>
+    <t>1964</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>1962</t>
+  </si>
+  <si>
+    <t>1961</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Hydro
+Power*</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>Capacity factor (excluding pumped hydro)</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1533,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1480,8 +1687,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF31393F"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1575,8 +1797,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1841,6 +2068,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFEAEAEA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFEAEAEA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1855,7 +2127,7 @@
     </xf>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2067,14 +2339,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2367,7 +2660,7 @@
       <selection activeCell="A22" sqref="A22:XFD26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
@@ -2605,7 +2898,7 @@
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75">
+    <row r="40" spans="1:3" ht="15.5">
       <c r="A40" s="24" t="s">
         <v>247</v>
       </c>
@@ -2645,12 +2938,12 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="30">
+    <row r="1" spans="1:33" ht="29">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -4880,12 +5173,12 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="30">
+    <row r="1" spans="1:33" ht="29">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -5391,131 +5684,131 @@
       </c>
       <c r="B5" s="5">
         <f>'BECF-pre-ret'!B5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="C5" s="5">
         <f>'BECF-pre-ret'!C5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="D5" s="5">
         <f>'BECF-pre-ret'!D5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="E5" s="5">
         <f>'BECF-pre-ret'!E5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="F5" s="5">
         <f>'BECF-pre-ret'!F5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="G5" s="5">
         <f>'BECF-pre-ret'!G5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="H5" s="5">
         <f>'BECF-pre-ret'!H5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="I5" s="5">
         <f>'BECF-pre-ret'!I5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="J5" s="5">
         <f>'BECF-pre-ret'!J5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="K5" s="5">
         <f>'BECF-pre-ret'!K5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="L5" s="5">
         <f>'BECF-pre-ret'!L5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="M5" s="5">
         <f>'BECF-pre-ret'!M5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="N5" s="5">
         <f>'BECF-pre-ret'!N5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="O5" s="5">
         <f>'BECF-pre-ret'!O5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="P5" s="5">
         <f>'BECF-pre-ret'!P5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="Q5" s="5">
         <f>'BECF-pre-ret'!Q5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="R5" s="5">
         <f>'BECF-pre-ret'!R5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="S5" s="5">
         <f>'BECF-pre-ret'!S5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="T5" s="5">
         <f>'BECF-pre-ret'!T5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="U5" s="5">
         <f>'BECF-pre-ret'!U5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="V5" s="5">
         <f>'BECF-pre-ret'!V5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="W5" s="5">
         <f>'BECF-pre-ret'!W5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="X5" s="5">
         <f>'BECF-pre-ret'!X5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="Y5" s="5">
         <f>'BECF-pre-ret'!Y5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="Z5" s="5">
         <f>'BECF-pre-ret'!Z5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AA5" s="5">
         <f>'BECF-pre-ret'!AA5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AB5" s="5">
         <f>'BECF-pre-ret'!AB5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AC5" s="5">
         <f>'BECF-pre-ret'!AC5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AD5" s="5">
         <f>'BECF-pre-ret'!AD5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AE5" s="5">
         <f>'BECF-pre-ret'!AE5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AF5" s="5">
         <f>'BECF-pre-ret'!AF5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AG5" s="5">
         <f>'BECF-pre-ret'!AG5</f>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -7129,9 +7422,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultColWidth="22.453125" defaultRowHeight="20.5"/>
   <cols>
-    <col min="1" max="16384" width="22.42578125" style="19"/>
+    <col min="1" max="16384" width="22.453125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="15" customFormat="1">
@@ -14496,10 +14789,10 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="1" max="3" width="23.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
@@ -14781,19 +15074,19 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" style="28" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="28" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="28" customWidth="1"/>
+    <col min="1" max="2" width="12.7265625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="28" customWidth="1"/>
     <col min="6" max="7" width="9" style="28"/>
-    <col min="8" max="8" width="25.5703125" style="28" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.54296875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="28" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A1" s="26" t="s">
         <v>252</v>
       </c>
@@ -14810,7 +15103,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A2" s="29" t="s">
         <v>256</v>
       </c>
@@ -14827,7 +15120,7 @@
         <v>11767747</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A3" s="31" t="s">
         <v>259</v>
       </c>
@@ -14847,7 +15140,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A4" s="31" t="s">
         <v>259</v>
       </c>
@@ -14881,7 +15174,7 @@
       <c r="P4" s="41"/>
       <c r="Q4" s="41"/>
     </row>
-    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A5" s="31" t="s">
         <v>259</v>
       </c>
@@ -14902,7 +15195,7 @@
       </c>
       <c r="I5" s="38"/>
     </row>
-    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A6" s="31" t="s">
         <v>259</v>
       </c>
@@ -14923,7 +15216,7 @@
       </c>
       <c r="I6" s="38"/>
     </row>
-    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A7" s="31" t="s">
         <v>259</v>
       </c>
@@ -14944,7 +15237,7 @@
       </c>
       <c r="I7" s="38"/>
     </row>
-    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A8" s="31" t="s">
         <v>259</v>
       </c>
@@ -14969,7 +15262,7 @@
       </c>
       <c r="L8" s="38"/>
     </row>
-    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A9" s="31" t="s">
         <v>259</v>
       </c>
@@ -14993,7 +15286,7 @@
         <v>11767747</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A10" s="31" t="s">
         <v>259</v>
       </c>
@@ -15014,7 +15307,7 @@
       </c>
       <c r="I10" s="38"/>
     </row>
-    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A11" s="31" t="s">
         <v>259</v>
       </c>
@@ -15038,7 +15331,7 @@
         <v>3141235</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A12" s="31" t="s">
         <v>259</v>
       </c>
@@ -15059,7 +15352,7 @@
       </c>
       <c r="I12" s="38"/>
     </row>
-    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A13" s="31" t="s">
         <v>259</v>
       </c>
@@ -15080,7 +15373,7 @@
       </c>
       <c r="I13" s="38"/>
     </row>
-    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A14" s="31" t="s">
         <v>259</v>
       </c>
@@ -15101,7 +15394,7 @@
       </c>
       <c r="I14" s="38"/>
     </row>
-    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A15" s="31" t="s">
         <v>259</v>
       </c>
@@ -15122,7 +15415,7 @@
       </c>
       <c r="I15" s="38"/>
     </row>
-    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A16" s="31" t="s">
         <v>259</v>
       </c>
@@ -15143,7 +15436,7 @@
       </c>
       <c r="I16" s="38"/>
     </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A17" s="31" t="s">
         <v>259</v>
       </c>
@@ -15164,7 +15457,7 @@
       </c>
       <c r="I17" s="38"/>
     </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A18" s="31" t="s">
         <v>259</v>
       </c>
@@ -15185,7 +15478,7 @@
       </c>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A19" s="31" t="s">
         <v>259</v>
       </c>
@@ -15209,7 +15502,7 @@
         <v>368170</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A20" s="31" t="s">
         <v>259</v>
       </c>
@@ -15226,7 +15519,7 @@
         <v>67820</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A21" s="31" t="s">
         <v>259</v>
       </c>
@@ -15243,7 +15536,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A22" s="31" t="s">
         <v>259</v>
       </c>
@@ -15260,7 +15553,7 @@
         <v>21999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A23" s="31" t="s">
         <v>259</v>
       </c>
@@ -15277,7 +15570,7 @@
         <v>21999</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A24" s="31" t="s">
         <v>259</v>
       </c>
@@ -15294,7 +15587,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A25" s="31" t="s">
         <v>259</v>
       </c>
@@ -15311,7 +15604,7 @@
         <v>1343074</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A26" s="31" t="s">
         <v>259</v>
       </c>
@@ -15328,7 +15621,7 @@
         <v>1343074</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A27" s="31" t="s">
         <v>259</v>
       </c>
@@ -15345,7 +15638,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A28" s="31" t="s">
         <v>259</v>
       </c>
@@ -15362,7 +15655,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A29" s="31" t="s">
         <v>259</v>
       </c>
@@ -15379,7 +15672,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A30" s="31" t="s">
         <v>259</v>
       </c>
@@ -15396,7 +15689,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A31" s="31" t="s">
         <v>259</v>
       </c>
@@ -15413,7 +15706,7 @@
         <v>36430</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A32" s="31" t="s">
         <v>259</v>
       </c>
@@ -15430,7 +15723,7 @@
         <v>36430</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A33" s="31" t="s">
         <v>259</v>
       </c>
@@ -15447,7 +15740,7 @@
         <v>140248</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A34" s="31" t="s">
         <v>259</v>
       </c>
@@ -15464,7 +15757,7 @@
         <v>140248</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A35" s="31" t="s">
         <v>259</v>
       </c>
@@ -15481,7 +15774,7 @@
         <v>450369</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A36" s="31" t="s">
         <v>259</v>
       </c>
@@ -15498,7 +15791,7 @@
         <v>450369</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A37" s="31" t="s">
         <v>259</v>
       </c>
@@ -15515,7 +15808,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A38" s="31" t="s">
         <v>259</v>
       </c>
@@ -15532,7 +15825,7 @@
         <v>1020350</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A39" s="31" t="s">
         <v>259</v>
       </c>
@@ -15549,7 +15842,7 @@
         <v>1020350</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A40" s="31" t="s">
         <v>259</v>
       </c>
@@ -15566,7 +15859,7 @@
         <v>368170</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A41" s="31" t="s">
         <v>259</v>
       </c>
@@ -15583,7 +15876,7 @@
         <v>284267</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A42" s="31" t="s">
         <v>259</v>
       </c>
@@ -15600,7 +15893,7 @@
         <v>83903</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A43" s="31" t="s">
         <v>259</v>
       </c>
@@ -15617,7 +15910,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A44" s="31" t="s">
         <v>259</v>
       </c>
@@ -15634,7 +15927,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A45" s="31" t="s">
         <v>259</v>
       </c>
@@ -15651,7 +15944,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A46" s="31" t="s">
         <v>259</v>
       </c>
@@ -15668,7 +15961,7 @@
         <v>100197</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A47" s="31" t="s">
         <v>259</v>
       </c>
@@ -15685,7 +15978,7 @@
         <v>94183</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A48" s="31" t="s">
         <v>259</v>
       </c>
@@ -15702,7 +15995,7 @@
         <v>6014</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="49" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A49" s="31" t="s">
         <v>259</v>
       </c>
@@ -15719,7 +16012,7 @@
         <v>120952</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="50" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A50" s="31" t="s">
         <v>259</v>
       </c>
@@ -15736,7 +16029,7 @@
         <v>50063</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="51" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A51" s="31" t="s">
         <v>259</v>
       </c>
@@ -15753,7 +16046,7 @@
         <v>70889</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="52" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A52" s="31" t="s">
         <v>259</v>
       </c>
@@ -15770,7 +16063,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="53" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A53" s="31" t="s">
         <v>259</v>
       </c>
@@ -15787,7 +16080,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="54" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A54" s="31" t="s">
         <v>259</v>
       </c>
@@ -15804,7 +16097,7 @@
         <v>147021</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="55" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A55" s="31" t="s">
         <v>259</v>
       </c>
@@ -15821,7 +16114,7 @@
         <v>140021</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="56" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A56" s="31" t="s">
         <v>259</v>
       </c>
@@ -15838,7 +16131,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A57" s="31" t="s">
         <v>259</v>
       </c>
@@ -15855,7 +16148,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="58" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A58" s="31" t="s">
         <v>259</v>
       </c>
@@ -15872,7 +16165,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="59" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A59" s="29" t="s">
         <v>285</v>
       </c>
@@ -15889,7 +16182,7 @@
         <v>469148</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="60" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A60" s="31" t="s">
         <v>259</v>
       </c>
@@ -15906,7 +16199,7 @@
         <v>464356</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="61" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A61" s="31" t="s">
         <v>259</v>
       </c>
@@ -15923,7 +16216,7 @@
         <v>4792</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="62" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A62" s="31" t="s">
         <v>259</v>
       </c>
@@ -15940,7 +16233,7 @@
         <v>346330</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="63" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A63" s="32" t="s">
         <v>259</v>
       </c>
@@ -15971,20 +16264,20 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="28" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="28" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="28" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="28" customWidth="1"/>
     <col min="6" max="7" width="9" style="28"/>
-    <col min="8" max="8" width="25.5703125" style="28" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.54296875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" style="28" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A1" s="26" t="s">
         <v>252</v>
       </c>
@@ -16001,7 +16294,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A2" s="29" t="s">
         <v>256</v>
       </c>
@@ -16018,7 +16311,7 @@
         <v>12996018</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A3" s="31" t="s">
         <v>259</v>
       </c>
@@ -16038,7 +16331,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A4" s="31" t="s">
         <v>259</v>
       </c>
@@ -16072,7 +16365,7 @@
       <c r="P4" s="41"/>
       <c r="Q4" s="41"/>
     </row>
-    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A5" s="31" t="s">
         <v>259</v>
       </c>
@@ -16093,7 +16386,7 @@
       </c>
       <c r="I5" s="38"/>
     </row>
-    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A6" s="31" t="s">
         <v>259</v>
       </c>
@@ -16114,7 +16407,7 @@
       </c>
       <c r="I6" s="38"/>
     </row>
-    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A7" s="31" t="s">
         <v>259</v>
       </c>
@@ -16135,7 +16428,7 @@
       </c>
       <c r="I7" s="38"/>
     </row>
-    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A8" s="31" t="s">
         <v>259</v>
       </c>
@@ -16159,7 +16452,7 @@
         <v>2679158</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A9" s="31" t="s">
         <v>259</v>
       </c>
@@ -16183,7 +16476,7 @@
         <v>12996018</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A10" s="31" t="s">
         <v>259</v>
       </c>
@@ -16204,7 +16497,7 @@
       </c>
       <c r="I10" s="38"/>
     </row>
-    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A11" s="31" t="s">
         <v>259</v>
       </c>
@@ -16228,7 +16521,7 @@
         <v>10415632</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A12" s="31" t="s">
         <v>259</v>
       </c>
@@ -16249,7 +16542,7 @@
       </c>
       <c r="I12" s="38"/>
     </row>
-    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A13" s="31" t="s">
         <v>259</v>
       </c>
@@ -16270,7 +16563,7 @@
       </c>
       <c r="I13" s="38"/>
     </row>
-    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A14" s="31" t="s">
         <v>259</v>
       </c>
@@ -16291,7 +16584,7 @@
       </c>
       <c r="I14" s="38"/>
     </row>
-    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A15" s="31" t="s">
         <v>259</v>
       </c>
@@ -16312,7 +16605,7 @@
       </c>
       <c r="I15" s="38"/>
     </row>
-    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:17" ht="20.149999999999999" customHeight="1">
       <c r="A16" s="31" t="s">
         <v>259</v>
       </c>
@@ -16333,7 +16626,7 @@
       </c>
       <c r="I16" s="38"/>
     </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A17" s="31" t="s">
         <v>259</v>
       </c>
@@ -16354,7 +16647,7 @@
       </c>
       <c r="I17" s="38"/>
     </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A18" s="31" t="s">
         <v>259</v>
       </c>
@@ -16375,7 +16668,7 @@
       </c>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A19" s="31" t="s">
         <v>259</v>
       </c>
@@ -16399,7 +16692,7 @@
         <v>356149</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A20" s="31" t="s">
         <v>259</v>
       </c>
@@ -16416,7 +16709,7 @@
         <v>239527</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A21" s="31" t="s">
         <v>259</v>
       </c>
@@ -16433,7 +16726,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A22" s="31" t="s">
         <v>259</v>
       </c>
@@ -16450,7 +16743,7 @@
         <v>41753</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A23" s="31" t="s">
         <v>259</v>
       </c>
@@ -16467,7 +16760,7 @@
         <v>41753</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A24" s="31" t="s">
         <v>259</v>
       </c>
@@ -16484,7 +16777,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A25" s="31" t="s">
         <v>259</v>
       </c>
@@ -16501,7 +16794,7 @@
         <v>4959229</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A26" s="31" t="s">
         <v>259</v>
       </c>
@@ -16518,7 +16811,7 @@
         <v>4959229</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A27" s="31" t="s">
         <v>259</v>
       </c>
@@ -16535,7 +16828,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A28" s="31" t="s">
         <v>259</v>
       </c>
@@ -16552,7 +16845,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A29" s="31" t="s">
         <v>259</v>
       </c>
@@ -16569,7 +16862,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A30" s="31" t="s">
         <v>259</v>
       </c>
@@ -16586,7 +16879,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A31" s="31" t="s">
         <v>259</v>
       </c>
@@ -16603,7 +16896,7 @@
         <v>277640</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:9" ht="20.149999999999999" customHeight="1">
       <c r="A32" s="31" t="s">
         <v>259</v>
       </c>
@@ -16620,7 +16913,7 @@
         <v>277640</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A33" s="31" t="s">
         <v>259</v>
       </c>
@@ -16637,7 +16930,7 @@
         <v>338143</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A34" s="31" t="s">
         <v>259</v>
       </c>
@@ -16654,7 +16947,7 @@
         <v>338143</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A35" s="31" t="s">
         <v>259</v>
       </c>
@@ -16671,7 +16964,7 @@
         <v>2068895</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A36" s="31" t="s">
         <v>259</v>
       </c>
@@ -16688,7 +16981,7 @@
         <v>2068895</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A37" s="31" t="s">
         <v>259</v>
       </c>
@@ -16705,7 +16998,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A38" s="31" t="s">
         <v>259</v>
       </c>
@@ -16722,7 +17015,7 @@
         <v>2295198</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A39" s="31" t="s">
         <v>259</v>
       </c>
@@ -16739,7 +17032,7 @@
         <v>2295198</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A40" s="31" t="s">
         <v>259</v>
       </c>
@@ -16756,7 +17049,7 @@
         <v>356149</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A41" s="31" t="s">
         <v>259</v>
       </c>
@@ -16773,7 +17066,7 @@
         <v>250856</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A42" s="31" t="s">
         <v>259</v>
       </c>
@@ -16790,7 +17083,7 @@
         <v>105293</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A43" s="31" t="s">
         <v>259</v>
       </c>
@@ -16807,7 +17100,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A44" s="31" t="s">
         <v>259</v>
       </c>
@@ -16824,7 +17117,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A45" s="31" t="s">
         <v>259</v>
       </c>
@@ -16841,7 +17134,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A46" s="31" t="s">
         <v>259</v>
       </c>
@@ -16858,7 +17151,7 @@
         <v>61302</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A47" s="31" t="s">
         <v>259</v>
       </c>
@@ -16875,7 +17168,7 @@
         <v>59646</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A48" s="31" t="s">
         <v>259</v>
       </c>
@@ -16892,7 +17185,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="49" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A49" s="31" t="s">
         <v>259</v>
       </c>
@@ -16909,7 +17202,7 @@
         <v>150081</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="50" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A50" s="31" t="s">
         <v>259</v>
       </c>
@@ -16926,7 +17219,7 @@
         <v>49971</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="51" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A51" s="31" t="s">
         <v>259</v>
       </c>
@@ -16943,7 +17236,7 @@
         <v>100110</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="52" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A52" s="31" t="s">
         <v>259</v>
       </c>
@@ -16960,7 +17253,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="53" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A53" s="31" t="s">
         <v>259</v>
       </c>
@@ -16977,7 +17270,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="54" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A54" s="31" t="s">
         <v>259</v>
       </c>
@@ -16994,7 +17287,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="55" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A55" s="31" t="s">
         <v>259</v>
       </c>
@@ -17011,7 +17304,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="56" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A56" s="31" t="s">
         <v>259</v>
       </c>
@@ -17028,7 +17321,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A57" s="31" t="s">
         <v>259</v>
       </c>
@@ -17045,7 +17338,7 @@
         <v>144766</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="58" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A58" s="31" t="s">
         <v>259</v>
       </c>
@@ -17062,7 +17355,7 @@
         <v>141239</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="59" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A59" s="31" t="s">
         <v>259</v>
       </c>
@@ -17079,7 +17372,7 @@
         <v>3527</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="60" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A60" s="31" t="s">
         <v>259</v>
       </c>
@@ -17096,7 +17389,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="61" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A61" s="31" t="s">
         <v>259</v>
       </c>
@@ -17113,7 +17406,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="62" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A62" s="31" t="s">
         <v>259</v>
       </c>
@@ -17130,7 +17423,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="63" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A63" s="31" t="s">
         <v>259</v>
       </c>
@@ -17147,7 +17440,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="64" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A64" s="29" t="s">
         <v>285</v>
       </c>
@@ -17164,7 +17457,7 @@
         <v>2285164</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="65" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A65" s="31" t="s">
         <v>259</v>
       </c>
@@ -17181,7 +17474,7 @@
         <v>2257401</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="66" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A66" s="31" t="s">
         <v>259</v>
       </c>
@@ -17198,7 +17491,7 @@
         <v>27764</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="67" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A67" s="31" t="s">
         <v>259</v>
       </c>
@@ -17215,7 +17508,7 @@
         <v>1031272</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="68" spans="1:5" ht="20.149999999999999" customHeight="1">
       <c r="A68" s="32" t="s">
         <v>259</v>
       </c>
@@ -17248,11 +17541,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="16.5" customHeight="1">
@@ -23966,16 +24259,16 @@
       <c r="AM72"/>
     </row>
     <row r="73" spans="1:62" s="46" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A73" s="117" t="s">
+      <c r="A73" s="119" t="s">
         <v>366</v>
       </c>
-      <c r="B73" s="117" t="s">
+      <c r="B73" s="119" t="s">
         <v>367</v>
       </c>
-      <c r="C73" s="117" t="s">
+      <c r="C73" s="119" t="s">
         <v>368</v>
       </c>
-      <c r="D73" s="117" t="s">
+      <c r="D73" s="119" t="s">
         <v>369</v>
       </c>
       <c r="E73"/>
@@ -24015,10 +24308,10 @@
       <c r="AM73"/>
     </row>
     <row r="74" spans="1:62" s="46" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A74" s="118"/>
-      <c r="B74" s="118"/>
-      <c r="C74" s="118"/>
-      <c r="D74" s="118"/>
+      <c r="A74" s="120"/>
+      <c r="B74" s="120"/>
+      <c r="C74" s="120"/>
+      <c r="D74" s="120"/>
       <c r="E74"/>
       <c r="F74"/>
       <c r="G74">
@@ -27698,12 +27991,1181 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C065EC5-E17F-471E-98A2-AE0C88E69387}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="5" width="8.7265625" style="125"/>
+    <col min="7" max="9" width="8.7265625" style="125"/>
+    <col min="12" max="12" width="12.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A1" s="121" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" s="121" t="s">
+        <v>410</v>
+      </c>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="G1" s="121" t="s">
+        <v>473</v>
+      </c>
+      <c r="H1" s="121" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" s="126"/>
+    </row>
+    <row r="2" spans="1:13" ht="87">
+      <c r="A2" s="121"/>
+      <c r="B2" s="122" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" s="122" t="s">
+        <v>412</v>
+      </c>
+      <c r="D2" s="122" t="s">
+        <v>413</v>
+      </c>
+      <c r="E2" s="122" t="s">
+        <v>391</v>
+      </c>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="122" t="s">
+        <v>474</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="M2">
+        <f>SUM(B3,D3)/(I4*8760)</f>
+        <v>0.24510682786539048</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16">
+      <c r="A3" s="123" t="s">
+        <v>414</v>
+      </c>
+      <c r="B3" s="124">
+        <v>3205979</v>
+      </c>
+      <c r="C3" s="124">
+        <v>3271019</v>
+      </c>
+      <c r="D3" s="124">
+        <v>671251</v>
+      </c>
+      <c r="E3" s="124">
+        <v>7148249</v>
+      </c>
+      <c r="G3" s="123" t="s">
+        <v>475</v>
+      </c>
+      <c r="H3" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I3" s="127">
+        <v>1841.1414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16">
+      <c r="A4" s="123" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="124">
+        <v>2229038.12</v>
+      </c>
+      <c r="C4" s="124">
+        <v>3458384.7549999999</v>
+      </c>
+      <c r="D4" s="124">
+        <v>559640.92709999997</v>
+      </c>
+      <c r="E4" s="124">
+        <v>6247063.8020000001</v>
+      </c>
+      <c r="G4" s="123" t="s">
+        <v>414</v>
+      </c>
+      <c r="H4" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I4" s="127">
+        <v>1805.7684000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16">
+      <c r="A5" s="123" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" s="124">
+        <v>2748401</v>
+      </c>
+      <c r="C5" s="124">
+        <v>3911035</v>
+      </c>
+      <c r="D5" s="124">
+        <v>611017</v>
+      </c>
+      <c r="E5" s="124">
+        <v>7270453</v>
+      </c>
+      <c r="G5" s="123" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I5" s="127">
+        <v>1808.1034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16">
+      <c r="A6" s="123" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6" s="124">
+        <v>2263505</v>
+      </c>
+      <c r="C6" s="124">
+        <v>4186353</v>
+      </c>
+      <c r="D6" s="124">
+        <v>545316</v>
+      </c>
+      <c r="E6" s="124">
+        <v>6995173</v>
+      </c>
+      <c r="G6" s="123" t="s">
+        <v>415</v>
+      </c>
+      <c r="H6" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I6" s="127">
+        <v>1790.4104000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16">
+      <c r="A7" s="123" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7" s="124">
+        <v>2159149</v>
+      </c>
+      <c r="C7" s="124">
+        <v>3787310</v>
+      </c>
+      <c r="D7" s="124">
+        <v>687112.6</v>
+      </c>
+      <c r="E7" s="124">
+        <v>6633585</v>
+      </c>
+      <c r="G7" s="123" t="s">
+        <v>416</v>
+      </c>
+      <c r="H7" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I7" s="127">
+        <v>1789.4560000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16">
+      <c r="A8" s="123" t="s">
+        <v>418</v>
+      </c>
+      <c r="B8" s="124">
+        <v>1539297.6850000001</v>
+      </c>
+      <c r="C8" s="124">
+        <v>3650320.3459999999</v>
+      </c>
+      <c r="D8" s="124">
+        <v>606421.62199999997</v>
+      </c>
+      <c r="E8" s="124">
+        <v>5796039.6519999998</v>
+      </c>
+      <c r="G8" s="123" t="s">
+        <v>417</v>
+      </c>
+      <c r="H8" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I8" s="127">
+        <v>1785.211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16">
+      <c r="A9" s="123" t="s">
+        <v>419</v>
+      </c>
+      <c r="B9" s="124">
+        <v>2135681</v>
+      </c>
+      <c r="C9" s="124">
+        <v>5068129</v>
+      </c>
+      <c r="D9" s="124">
+        <v>615737</v>
+      </c>
+      <c r="E9" s="124">
+        <v>7819548</v>
+      </c>
+      <c r="G9" s="123" t="s">
+        <v>418</v>
+      </c>
+      <c r="H9" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I9" s="127">
+        <v>1770.7090000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16">
+      <c r="A10" s="123" t="s">
+        <v>420</v>
+      </c>
+      <c r="B10" s="124">
+        <v>3798240</v>
+      </c>
+      <c r="C10" s="124">
+        <v>4104661</v>
+      </c>
+      <c r="D10" s="124">
+        <v>491028</v>
+      </c>
+      <c r="E10" s="124">
+        <v>8393928</v>
+      </c>
+      <c r="G10" s="123" t="s">
+        <v>419</v>
+      </c>
+      <c r="H10" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I10" s="127">
+        <v>1766.9359999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16">
+      <c r="A11" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="B11" s="124">
+        <v>3440018</v>
+      </c>
+      <c r="C11" s="124">
+        <v>3683262</v>
+      </c>
+      <c r="D11" s="124">
+        <v>529021</v>
+      </c>
+      <c r="E11" s="124">
+        <v>7652301</v>
+      </c>
+      <c r="G11" s="123" t="s">
+        <v>420</v>
+      </c>
+      <c r="H11" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I11" s="127">
+        <v>1754.4620000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16">
+      <c r="A12" s="123" t="s">
+        <v>422</v>
+      </c>
+      <c r="B12" s="124">
+        <v>4178867.7</v>
+      </c>
+      <c r="C12" s="124">
+        <v>3232984.5729999999</v>
+      </c>
+      <c r="D12" s="124">
+        <v>418799.31599999999</v>
+      </c>
+      <c r="E12" s="124">
+        <v>7830651.5889999997</v>
+      </c>
+      <c r="G12" s="123" t="s">
+        <v>421</v>
+      </c>
+      <c r="H12" s="127">
+        <v>4700</v>
+      </c>
+      <c r="I12" s="127">
+        <v>1746.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16">
+      <c r="A13" s="123" t="s">
+        <v>423</v>
+      </c>
+      <c r="B13" s="124">
+        <v>3339560.27</v>
+      </c>
+      <c r="C13" s="124">
+        <v>2789933.7510000002</v>
+      </c>
+      <c r="D13" s="124">
+        <v>342408.51299999998</v>
+      </c>
+      <c r="E13" s="124">
+        <v>6471902.534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16">
+      <c r="A14" s="123" t="s">
+        <v>424</v>
+      </c>
+      <c r="B14" s="124">
+        <v>2596099.9679999999</v>
+      </c>
+      <c r="C14" s="124">
+        <v>2827990.827</v>
+      </c>
+      <c r="D14" s="124">
+        <v>217071.277</v>
+      </c>
+      <c r="E14" s="124">
+        <v>5641162.0719999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16">
+      <c r="A15" s="123" t="s">
+        <v>425</v>
+      </c>
+      <c r="B15" s="124">
+        <v>2852126.8620000002</v>
+      </c>
+      <c r="C15" s="124">
+        <v>2492539.199</v>
+      </c>
+      <c r="D15" s="124">
+        <v>217984.48499999999</v>
+      </c>
+      <c r="E15" s="124">
+        <v>5562650.5460000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16">
+      <c r="A16" s="123" t="s">
+        <v>426</v>
+      </c>
+      <c r="B16" s="124">
+        <v>3475268.6529999999</v>
+      </c>
+      <c r="C16" s="124">
+        <v>1410812.7860000001</v>
+      </c>
+      <c r="D16" s="124">
+        <v>156380.554</v>
+      </c>
+      <c r="E16" s="124">
+        <v>5042461.9929999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16">
+      <c r="A17" s="123" t="s">
+        <v>427</v>
+      </c>
+      <c r="B17" s="124">
+        <v>3326281.3670000001</v>
+      </c>
+      <c r="C17" s="124">
+        <v>1751083.2549999999</v>
+      </c>
+      <c r="D17" s="124">
+        <v>141256.46</v>
+      </c>
+      <c r="E17" s="124">
+        <v>5218621.0820000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16">
+      <c r="A18" s="123" t="s">
+        <v>428</v>
+      </c>
+      <c r="B18" s="124">
+        <v>3535571.4380000001</v>
+      </c>
+      <c r="C18" s="124">
+        <v>1515588.405</v>
+      </c>
+      <c r="D18" s="124">
+        <v>137728.54399999999</v>
+      </c>
+      <c r="E18" s="124">
+        <v>5188888.3870000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16">
+      <c r="A19" s="123" t="s">
+        <v>429</v>
+      </c>
+      <c r="B19" s="124">
+        <v>4198348.0630000001</v>
+      </c>
+      <c r="C19" s="124">
+        <v>1550354.8</v>
+      </c>
+      <c r="D19" s="124">
+        <v>112731.63499999999</v>
+      </c>
+      <c r="E19" s="124">
+        <v>5861434.4979999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" s="123" t="s">
+        <v>430</v>
+      </c>
+      <c r="B20" s="124">
+        <v>4756941.3600000003</v>
+      </c>
+      <c r="C20" s="124">
+        <v>2001406.486</v>
+      </c>
+      <c r="D20" s="124">
+        <v>128635.63</v>
+      </c>
+      <c r="E20" s="124">
+        <v>6886983.4759999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16">
+      <c r="A21" s="123" t="s">
+        <v>431</v>
+      </c>
+      <c r="B21" s="124">
+        <v>3136673.9730000002</v>
+      </c>
+      <c r="C21" s="124">
+        <v>2078269.2</v>
+      </c>
+      <c r="D21" s="124">
+        <v>96103.335000000006</v>
+      </c>
+      <c r="E21" s="124">
+        <v>5311046.5080000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16">
+      <c r="A22" s="123" t="s">
+        <v>432</v>
+      </c>
+      <c r="B22" s="124">
+        <v>2257584.7110000001</v>
+      </c>
+      <c r="C22" s="124">
+        <v>1820814.209</v>
+      </c>
+      <c r="D22" s="124">
+        <v>72354.051999999996</v>
+      </c>
+      <c r="E22" s="124">
+        <v>4150752.9720000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16">
+      <c r="A23" s="123" t="s">
+        <v>433</v>
+      </c>
+      <c r="B23" s="124">
+        <v>3941017.4</v>
+      </c>
+      <c r="C23" s="124">
+        <v>1600269</v>
+      </c>
+      <c r="D23" s="124">
+        <v>68535.600000000006</v>
+      </c>
+      <c r="E23" s="124">
+        <v>5609822</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16">
+      <c r="A24" s="123" t="s">
+        <v>434</v>
+      </c>
+      <c r="B24" s="124">
+        <v>4068660</v>
+      </c>
+      <c r="C24" s="124">
+        <v>1906973</v>
+      </c>
+      <c r="D24" s="124">
+        <v>90600</v>
+      </c>
+      <c r="E24" s="124">
+        <v>6066233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16">
+      <c r="A25" s="123" t="s">
+        <v>435</v>
+      </c>
+      <c r="B25" s="124">
+        <v>4186592</v>
+      </c>
+      <c r="C25" s="124">
+        <v>1819618</v>
+      </c>
+      <c r="D25" s="124">
+        <v>92826</v>
+      </c>
+      <c r="E25" s="124">
+        <v>6099036</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16">
+      <c r="A26" s="123" t="s">
+        <v>436</v>
+      </c>
+      <c r="B26" s="124">
+        <v>2737161</v>
+      </c>
+      <c r="C26" s="124">
+        <v>2589533</v>
+      </c>
+      <c r="D26" s="124">
+        <v>76831</v>
+      </c>
+      <c r="E26" s="124">
+        <v>5403525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16">
+      <c r="A27" s="123" t="s">
+        <v>437</v>
+      </c>
+      <c r="B27" s="124">
+        <v>2353688</v>
+      </c>
+      <c r="C27" s="124">
+        <v>2776967</v>
+      </c>
+      <c r="D27" s="124">
+        <v>70669</v>
+      </c>
+      <c r="E27" s="124">
+        <v>5201324</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16">
+      <c r="A28" s="123" t="s">
+        <v>438</v>
+      </c>
+      <c r="B28" s="124">
+        <v>2689336</v>
+      </c>
+      <c r="C28" s="124">
+        <v>2717995</v>
+      </c>
+      <c r="D28" s="124">
+        <v>70587</v>
+      </c>
+      <c r="E28" s="124">
+        <v>5477918</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16">
+      <c r="A29" s="123" t="s">
+        <v>439</v>
+      </c>
+      <c r="B29" s="124">
+        <v>2266913</v>
+      </c>
+      <c r="C29" s="124">
+        <v>1752160</v>
+      </c>
+      <c r="D29" s="124">
+        <v>79179</v>
+      </c>
+      <c r="E29" s="124">
+        <v>4098252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16">
+      <c r="A30" s="123" t="s">
+        <v>440</v>
+      </c>
+      <c r="B30" s="124">
+        <v>4132212</v>
+      </c>
+      <c r="C30" s="124">
+        <v>1778530</v>
+      </c>
+      <c r="D30" s="124">
+        <v>95337</v>
+      </c>
+      <c r="E30" s="124">
+        <v>6006079</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16">
+      <c r="A31" s="123" t="s">
+        <v>441</v>
+      </c>
+      <c r="B31" s="124">
+        <v>3016042</v>
+      </c>
+      <c r="C31" s="124">
+        <v>1765775</v>
+      </c>
+      <c r="D31" s="124">
+        <v>81406</v>
+      </c>
+      <c r="E31" s="124">
+        <v>4863223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16">
+      <c r="A32" s="123" t="s">
+        <v>442</v>
+      </c>
+      <c r="B32" s="124">
+        <v>3458592</v>
+      </c>
+      <c r="C32" s="124">
+        <v>1564686</v>
+      </c>
+      <c r="D32" s="124">
+        <v>27454</v>
+      </c>
+      <c r="E32" s="124">
+        <v>5050732</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16">
+      <c r="A33" s="123" t="s">
+        <v>443</v>
+      </c>
+      <c r="B33" s="124">
+        <v>4605798</v>
+      </c>
+      <c r="C33" s="124">
+        <v>1677407</v>
+      </c>
+      <c r="D33" s="124">
+        <v>78148</v>
+      </c>
+      <c r="E33" s="124">
+        <v>6361353</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16">
+      <c r="A34" s="123" t="s">
+        <v>444</v>
+      </c>
+      <c r="B34" s="124">
+        <v>2896415</v>
+      </c>
+      <c r="C34" s="124">
+        <v>1593981</v>
+      </c>
+      <c r="D34" s="124">
+        <v>67554</v>
+      </c>
+      <c r="E34" s="124">
+        <v>4557950</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16">
+      <c r="A35" s="123" t="s">
+        <v>445</v>
+      </c>
+      <c r="B35" s="124">
+        <v>1956384</v>
+      </c>
+      <c r="C35" s="124">
+        <v>1578844</v>
+      </c>
+      <c r="D35" s="124">
+        <v>30848</v>
+      </c>
+      <c r="E35" s="124">
+        <v>3566076</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16">
+      <c r="A36" s="123" t="s">
+        <v>446</v>
+      </c>
+      <c r="B36" s="124">
+        <v>3924871</v>
+      </c>
+      <c r="C36" s="124">
+        <v>1378825</v>
+      </c>
+      <c r="D36" s="124">
+        <v>40500</v>
+      </c>
+      <c r="E36" s="124">
+        <v>5344196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16">
+      <c r="A37" s="123" t="s">
+        <v>447</v>
+      </c>
+      <c r="B37" s="124">
+        <v>3082265</v>
+      </c>
+      <c r="C37" s="124">
+        <v>909501</v>
+      </c>
+      <c r="D37" s="124">
+        <v>27615</v>
+      </c>
+      <c r="E37" s="124">
+        <v>4019381</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16">
+      <c r="A38" s="123" t="s">
+        <v>448</v>
+      </c>
+      <c r="B38" s="124">
+        <v>3165026</v>
+      </c>
+      <c r="C38" s="124">
+        <v>474114</v>
+      </c>
+      <c r="D38" s="124">
+        <v>19940</v>
+      </c>
+      <c r="E38" s="124">
+        <v>3659080</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16">
+      <c r="A39" s="123" t="s">
+        <v>449</v>
+      </c>
+      <c r="B39" s="124">
+        <v>1998143</v>
+      </c>
+      <c r="C39" s="124">
+        <v>400592</v>
+      </c>
+      <c r="D39" s="124">
+        <v>0</v>
+      </c>
+      <c r="E39" s="124">
+        <v>2398735</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16">
+      <c r="A40" s="123" t="s">
+        <v>450</v>
+      </c>
+      <c r="B40" s="124">
+        <v>2294191</v>
+      </c>
+      <c r="C40" s="124">
+        <v>428426</v>
+      </c>
+      <c r="D40" s="124">
+        <v>0</v>
+      </c>
+      <c r="E40" s="124">
+        <v>2722617</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16">
+      <c r="A41" s="123" t="s">
+        <v>451</v>
+      </c>
+      <c r="B41" s="124">
+        <v>1715362</v>
+      </c>
+      <c r="C41" s="124">
+        <v>289888</v>
+      </c>
+      <c r="D41" s="124">
+        <v>0</v>
+      </c>
+      <c r="E41" s="124">
+        <v>2005250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16">
+      <c r="A42" s="123" t="s">
+        <v>452</v>
+      </c>
+      <c r="B42" s="124">
+        <v>2597707</v>
+      </c>
+      <c r="C42" s="124">
+        <v>110823</v>
+      </c>
+      <c r="D42" s="124">
+        <v>0</v>
+      </c>
+      <c r="E42" s="124">
+        <v>2708530</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16">
+      <c r="A43" s="123" t="s">
+        <v>453</v>
+      </c>
+      <c r="B43" s="124">
+        <v>1920375</v>
+      </c>
+      <c r="C43" s="124">
+        <v>63716</v>
+      </c>
+      <c r="D43" s="124">
+        <v>0</v>
+      </c>
+      <c r="E43" s="124">
+        <v>1984091</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16">
+      <c r="A44" s="123" t="s">
+        <v>454</v>
+      </c>
+      <c r="B44" s="124">
+        <v>2296168</v>
+      </c>
+      <c r="C44" s="124">
+        <v>32361</v>
+      </c>
+      <c r="D44" s="124">
+        <v>0</v>
+      </c>
+      <c r="E44" s="124">
+        <v>2328529</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16">
+      <c r="A45" s="123" t="s">
+        <v>455</v>
+      </c>
+      <c r="B45" s="124">
+        <v>1807524</v>
+      </c>
+      <c r="C45" s="124">
+        <v>0</v>
+      </c>
+      <c r="D45" s="124">
+        <v>0</v>
+      </c>
+      <c r="E45" s="124">
+        <v>1807524</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16">
+      <c r="A46" s="123" t="s">
+        <v>456</v>
+      </c>
+      <c r="B46" s="124">
+        <v>1392729</v>
+      </c>
+      <c r="C46" s="124">
+        <v>0</v>
+      </c>
+      <c r="D46" s="124">
+        <v>0</v>
+      </c>
+      <c r="E46" s="124">
+        <v>1392729</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16">
+      <c r="A47" s="123" t="s">
+        <v>457</v>
+      </c>
+      <c r="B47" s="124">
+        <v>1788661</v>
+      </c>
+      <c r="C47" s="124">
+        <v>0</v>
+      </c>
+      <c r="D47" s="124">
+        <v>0</v>
+      </c>
+      <c r="E47" s="124">
+        <v>1788661</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="16">
+      <c r="A48" s="123" t="s">
+        <v>458</v>
+      </c>
+      <c r="B48" s="124">
+        <v>1682809</v>
+      </c>
+      <c r="C48" s="124">
+        <v>0</v>
+      </c>
+      <c r="D48" s="124">
+        <v>0</v>
+      </c>
+      <c r="E48" s="124">
+        <v>1682809</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="16">
+      <c r="A49" s="123" t="s">
+        <v>459</v>
+      </c>
+      <c r="B49" s="124">
+        <v>1905858</v>
+      </c>
+      <c r="C49" s="124">
+        <v>0</v>
+      </c>
+      <c r="D49" s="124">
+        <v>0</v>
+      </c>
+      <c r="E49" s="124">
+        <v>1905858</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="16">
+      <c r="A50" s="123" t="s">
+        <v>460</v>
+      </c>
+      <c r="B50" s="124">
+        <v>1284465</v>
+      </c>
+      <c r="C50" s="124">
+        <v>0</v>
+      </c>
+      <c r="D50" s="124">
+        <v>0</v>
+      </c>
+      <c r="E50" s="124">
+        <v>1284465</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="16">
+      <c r="A51" s="123" t="s">
+        <v>461</v>
+      </c>
+      <c r="B51" s="124">
+        <v>1368076</v>
+      </c>
+      <c r="C51" s="124">
+        <v>0</v>
+      </c>
+      <c r="D51" s="124">
+        <v>0</v>
+      </c>
+      <c r="E51" s="124">
+        <v>1368076</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="16">
+      <c r="A52" s="123" t="s">
+        <v>462</v>
+      </c>
+      <c r="B52" s="124">
+        <v>1319976</v>
+      </c>
+      <c r="C52" s="124">
+        <v>0</v>
+      </c>
+      <c r="D52" s="124">
+        <v>0</v>
+      </c>
+      <c r="E52" s="124">
+        <v>1319976</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="16">
+      <c r="A53" s="123" t="s">
+        <v>463</v>
+      </c>
+      <c r="B53" s="124">
+        <v>1220684</v>
+      </c>
+      <c r="C53" s="124">
+        <v>0</v>
+      </c>
+      <c r="D53" s="124">
+        <v>0</v>
+      </c>
+      <c r="E53" s="124">
+        <v>1220684</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16">
+      <c r="A54" s="123" t="s">
+        <v>464</v>
+      </c>
+      <c r="B54" s="124">
+        <v>1428512</v>
+      </c>
+      <c r="C54" s="124">
+        <v>0</v>
+      </c>
+      <c r="D54" s="124">
+        <v>0</v>
+      </c>
+      <c r="E54" s="124">
+        <v>1428512</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="16">
+      <c r="A55" s="123" t="s">
+        <v>465</v>
+      </c>
+      <c r="B55" s="124">
+        <v>929483</v>
+      </c>
+      <c r="C55" s="124">
+        <v>0</v>
+      </c>
+      <c r="D55" s="124">
+        <v>0</v>
+      </c>
+      <c r="E55" s="124">
+        <v>929483</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="16">
+      <c r="A56" s="123" t="s">
+        <v>466</v>
+      </c>
+      <c r="B56" s="124">
+        <v>953171</v>
+      </c>
+      <c r="C56" s="124">
+        <v>0</v>
+      </c>
+      <c r="D56" s="124">
+        <v>0</v>
+      </c>
+      <c r="E56" s="124">
+        <v>953171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="16">
+      <c r="A57" s="123" t="s">
+        <v>467</v>
+      </c>
+      <c r="B57" s="124">
+        <v>985322</v>
+      </c>
+      <c r="C57" s="124">
+        <v>0</v>
+      </c>
+      <c r="D57" s="124">
+        <v>0</v>
+      </c>
+      <c r="E57" s="124">
+        <v>985322</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="16">
+      <c r="A58" s="123" t="s">
+        <v>468</v>
+      </c>
+      <c r="B58" s="124">
+        <v>710427</v>
+      </c>
+      <c r="C58" s="124">
+        <v>0</v>
+      </c>
+      <c r="D58" s="124">
+        <v>0</v>
+      </c>
+      <c r="E58" s="124">
+        <v>710427</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="16">
+      <c r="A59" s="123" t="s">
+        <v>469</v>
+      </c>
+      <c r="B59" s="124">
+        <v>749905</v>
+      </c>
+      <c r="C59" s="124">
+        <v>0</v>
+      </c>
+      <c r="D59" s="124">
+        <v>0</v>
+      </c>
+      <c r="E59" s="124">
+        <v>749905</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="16">
+      <c r="A60" s="123" t="s">
+        <v>470</v>
+      </c>
+      <c r="B60" s="124">
+        <v>727829</v>
+      </c>
+      <c r="C60" s="124">
+        <v>0</v>
+      </c>
+      <c r="D60" s="124">
+        <v>0</v>
+      </c>
+      <c r="E60" s="124">
+        <v>727829</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="16">
+      <c r="A61" s="123" t="s">
+        <v>471</v>
+      </c>
+      <c r="B61" s="124">
+        <v>702341</v>
+      </c>
+      <c r="C61" s="124">
+        <v>0</v>
+      </c>
+      <c r="D61" s="124">
+        <v>0</v>
+      </c>
+      <c r="E61" s="124">
+        <v>702341</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="16">
+      <c r="A62" s="123" t="s">
+        <v>472</v>
+      </c>
+      <c r="B62" s="124">
+        <v>652611</v>
+      </c>
+      <c r="C62" s="124">
+        <v>0</v>
+      </c>
+      <c r="D62" s="124">
+        <v>0</v>
+      </c>
+      <c r="E62" s="124">
+        <v>652611</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -27719,11 +29181,11 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="4" width="23.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:5">
@@ -28027,18 +29489,18 @@
   </sheetPr>
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="30">
+    <row r="1" spans="1:33" ht="29">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -28543,132 +30005,132 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <f>StartYear_cal!E8</f>
-        <v>0.15532142169478805</v>
+        <f>Hydro!M2</f>
+        <v>0.24510682786539048</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="N5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="P5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="Q5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="R5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="S5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="T5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="U5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="V5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="W5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="X5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="Y5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="Z5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AA5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AB5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AC5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AD5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AE5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AF5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
       <c r="AG5" s="5">
         <f t="shared" si="0"/>
-        <v>0.15532142169478805</v>
+        <v>0.24510682786539048</v>
       </c>
     </row>
     <row r="6" spans="1:33">
@@ -29739,7 +31201,7 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="120">
+      <c r="B14" s="118">
         <v>0.3</v>
       </c>
       <c r="C14" s="5">
@@ -30274,10 +31736,10 @@
       <c r="D19" s="87"/>
     </row>
     <row r="20" spans="1:33">
-      <c r="B20" s="119" t="s">
+      <c r="B20" s="117" t="s">
         <v>408</v>
       </c>
-      <c r="C20" s="119"/>
+      <c r="C20" s="117"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>